<commit_message>
TestNg suite file changes
</commit_message>
<xml_diff>
--- a/target/classes/com/demo/automation/POMFramework/data/TestData.xlsx
+++ b/target/classes/com/demo/automation/POMFramework/data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1215" windowWidth="14295" windowHeight="3540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="1215" windowWidth="19815" windowHeight="3540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>userName</t>
   </si>
@@ -34,9 +34,6 @@
     <t>runMode</t>
   </si>
   <si>
-    <t>automation@gmail.com</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
@@ -47,6 +44,24 @@
   </si>
   <si>
     <t>12345678</t>
+  </si>
+  <si>
+    <t>jakay11@gmail.com</t>
+  </si>
+  <si>
+    <t>jakay12@gmail.com</t>
+  </si>
+  <si>
+    <t>jakay13@gmail.com</t>
+  </si>
+  <si>
+    <t>jakay14@gmail.com</t>
+  </si>
+  <si>
+    <t>jakay15@gmail.com</t>
+  </si>
+  <si>
+    <t>jakay16@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -380,7 +395,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -391,7 +406,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -412,90 +427,90 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>12345678</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>12345678</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>12345678</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>12345678</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>12345678</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>12345678</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A8" r:id="rId2"/>
+    <hyperlink ref="A6" r:id="rId3"/>
+    <hyperlink ref="A7" r:id="rId4"/>
+    <hyperlink ref="A3" r:id="rId5"/>
+    <hyperlink ref="A4" r:id="rId6"/>
+    <hyperlink ref="A5" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>